<commit_message>
updated xcms with command line test version
</commit_message>
<xml_diff>
--- a/xcms.xlsx
+++ b/xcms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gkreder/Library/Caches/Transmit/F66CD55E-A393-410A-9CE1-AB132673B11E/192.168.1.78/home/gkreder/scripts/PyMetab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gkreder/Library/Caches/Transmit/4B0A2991-3896-426A-92E7-7382E57E199E/69.209.6.213/home/gkreder/scripts/PyMetab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132F48DA-673C-CA46-B310-BB3544E5EB93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9BE595-9881-B540-8E7B-6E899C22B6AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20540" xr2:uid="{2B4E802A-F725-1847-85BF-4E53BE1B7AE8}"/>
+    <workbookView xWindow="18400" yWindow="-28340" windowWidth="25600" windowHeight="28340" xr2:uid="{2B4E802A-F725-1847-85BF-4E53BE1B7AE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>in_files</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>./data/XCMSnEXP.tsv</t>
+  </si>
+  <si>
+    <t>grouping_steps</t>
   </si>
 </sst>
 </file>
@@ -475,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2857AAC6-0935-D84F-A066-0FB3B99BD368}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -686,6 +689,14 @@
         <v>200</v>
       </c>
     </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>